<commit_message>
SStudy files and paper prototypes
</commit_message>
<xml_diff>
--- a/Studies/Demographic Questionnares/DemographicDetails.xlsx
+++ b/Studies/Demographic Questionnares/DemographicDetails.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="63">
   <si>
     <t>Participant Demographic Questionnare Details</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Iphone, Ipad</t>
+  </si>
+  <si>
+    <t>Samsung Notebook 10.1 Pro</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,6 +1185,50 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" t="s">
+        <v>62</v>
+      </c>
+      <c r="P15" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:L1"/>

</xml_diff>